<commit_message>
Update on status of the project
</commit_message>
<xml_diff>
--- a/NewAgeDating2/Status_of_project.xlsx
+++ b/NewAgeDating2/Status_of_project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Authentication</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Additions Features to Work on?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to Modularize error responses </t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +104,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -114,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -124,6 +133,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +431,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="A1:XFD1048576"/>
+      <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,6 +480,9 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>